<commit_message>
Modified Excel - No conflict check
</commit_message>
<xml_diff>
--- a/src/test/resources/NewExcel.xlsx
+++ b/src/test/resources/NewExcel.xlsx
@@ -1,51 +1,46 @@
 
-<file path=docProps\app.xml><?xml version="1.0" encoding="utf-8"?>
-<Properties xmlns="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <Application>Microsoft Excel</Application>
-  <DocSecurity>0</DocSecurity>
-  <ScaleCrop>false</ScaleCrop>
-  <HeadingPairs>
-    <vt:vector size="2" baseType="variant">
-      <vt:variant>
-        <vt:lpstr>Worksheets</vt:lpstr>
-      </vt:variant>
-      <vt:variant>
-        <vt:i4>10</vt:i4>
-      </vt:variant>
-    </vt:vector>
-  </HeadingPairs>
-  <TitlesOfParts>
-    <vt:vector size="10" baseType="lpstr">
-      <vt:lpstr>Amazon</vt:lpstr>
-      <vt:lpstr>SecurityPage</vt:lpstr>
-      <vt:lpstr>NameChange</vt:lpstr>
-      <vt:lpstr>AccountPage</vt:lpstr>
-      <vt:lpstr>SearchPage</vt:lpstr>
-      <vt:lpstr>ProductPage</vt:lpstr>
-      <vt:lpstr>OrderCartPage</vt:lpstr>
-      <vt:lpstr>LoginPage</vt:lpstr>
-      <vt:lpstr>CheckOutPage</vt:lpstr>
-      <vt:lpstr>Results</vt:lpstr>
-    </vt:vector>
-  </TitlesOfParts>
-  <LinksUpToDate>false</LinksUpToDate>
-  <SharedDoc>false</SharedDoc>
-  <HyperlinksChanged>false</HyperlinksChanged>
-  <AppVersion>16.0300</AppVersion>
-</Properties>
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UB217ZA\Downloads\excel-version-control\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BBB0FC-574D-4E53-93CA-4F2E32D7A538}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Amazon" sheetId="1" r:id="rId1"/>
+    <sheet name="SecurityPage" sheetId="2" r:id="rId2"/>
+    <sheet name="NameChange" sheetId="3" r:id="rId3"/>
+    <sheet name="AccountPage" sheetId="4" r:id="rId4"/>
+    <sheet name="SearchPage" sheetId="5" r:id="rId5"/>
+    <sheet name="ProductPage" sheetId="6" r:id="rId6"/>
+    <sheet name="OrderCartPage" sheetId="7" r:id="rId7"/>
+    <sheet name="LoginPage" sheetId="8" r:id="rId8"/>
+    <sheet name="CheckOutPage" sheetId="9" r:id="rId9"/>
+    <sheet name="Results" sheetId="10" r:id="rId10"/>
+  </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
+</workbook>
 </file>
 
-<file path=docProps\core.xml><?xml version="1.0" encoding="utf-8"?>
-<cp:coreProperties xmlns:cp="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:dcmitype="http://purl.org/dc/dcmitype/" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <dc:creator>Macharla, Pradeep</dc:creator>
-  <cp:lastModifiedBy>Divya M</cp:lastModifiedBy>
-  <dcterms:created xsi:type="dcterms:W3CDTF">2014-12-07T20:26:11Z</dcterms:created>
-  <dcterms:modified xsi:type="dcterms:W3CDTF">2022-04-18T13:50:43Z</dcterms:modified>
-</cp:coreProperties>
-</file>
-
-<file path=xl\sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="158">
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="158">
   <si>
     <t>element_type</t>
   </si>
@@ -518,12 +513,12 @@
     <t>twotabsearchtextbox</t>
   </si>
   <si>
-    <t>home</t>
+    <t>home_1</t>
   </si>
 </sst>
 </file>
 
-<file path=xl\styles.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -573,7 +568,7 @@
 </styleSheet>
 </file>
 
-<file path=xl\theme\theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
@@ -892,47 +887,7 @@
 </a:theme>
 </file>
 
-<file path=xl\workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UB217ZA\Downloads\Github Clone NGTP\excel-version-control\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDB18B1-E140-44B8-8466-F756747AC1AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Amazon" sheetId="1" r:id="rId1"/>
-    <sheet name="SecurityPage" sheetId="2" r:id="rId2"/>
-    <sheet name="NameChange" sheetId="3" r:id="rId3"/>
-    <sheet name="AccountPage" sheetId="4" r:id="rId4"/>
-    <sheet name="SearchPage" sheetId="5" r:id="rId5"/>
-    <sheet name="ProductPage" sheetId="6" r:id="rId6"/>
-    <sheet name="OrderCartPage" sheetId="7" r:id="rId7"/>
-    <sheet name="LoginPage" sheetId="8" r:id="rId8"/>
-    <sheet name="CheckOutPage" sheetId="9" r:id="rId9"/>
-    <sheet name="Results" sheetId="10" r:id="rId10"/>
-  </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
-</workbook>
-</file>
-
-<file path=xl\worksheets\sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
@@ -1059,6 +1014,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
       <c r="B11" t="s">
         <v>29</v>
       </c>
@@ -1094,12 +1052,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:F1 A4:F14 A3:C3 E3:F3 A2 C2:D2 F2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:F1 A4:F9 A3:C3 E3:F3 A2 C2:D2 F2 A12:F14 B10:F10 B11:F11" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl\worksheets\sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -1162,7 +1120,7 @@
 </worksheet>
 </file>
 
-<file path=xl\worksheets\sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
@@ -1246,7 +1204,7 @@
 </worksheet>
 </file>
 
-<file path=xl\worksheets\sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -1322,7 +1280,7 @@
 </worksheet>
 </file>
 
-<file path=xl\worksheets\sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -1382,7 +1340,7 @@
 </worksheet>
 </file>
 
-<file path=xl\worksheets\sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
@@ -1513,7 +1471,7 @@
 </worksheet>
 </file>
 
-<file path=xl\worksheets\sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
@@ -1746,7 +1704,7 @@
 </worksheet>
 </file>
 
-<file path=xl\worksheets\sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
@@ -1866,7 +1824,7 @@
 </worksheet>
 </file>
 
-<file path=xl\worksheets\sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
@@ -2005,7 +1963,7 @@
 </worksheet>
 </file>
 
-<file path=xl\worksheets\sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>

</xml_diff>

<commit_message>
Modified Excel - 1 - To check conflict
</commit_message>
<xml_diff>
--- a/src/test/resources/NewExcel.xlsx
+++ b/src/test/resources/NewExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UB217ZA\Downloads\excel-version-control\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BBB0FC-574D-4E53-93CA-4F2E32D7A538}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99585037-83FB-47A4-98E5-B83A8595DB1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -513,7 +513,7 @@
     <t>twotabsearchtextbox</t>
   </si>
   <si>
-    <t>home_1</t>
+    <t>home_2</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Modified Excel - 2 - To check conflict
</commit_message>
<xml_diff>
--- a/src/test/resources/NewExcel.xlsx
+++ b/src/test/resources/NewExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UB217ZA\Downloads\excel-version-control\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BBB0FC-574D-4E53-93CA-4F2E32D7A538}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23717606-8151-459B-9E64-A7434E713B22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -513,7 +513,7 @@
     <t>twotabsearchtextbox</t>
   </si>
   <si>
-    <t>home_1</t>
+    <t>home_3</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Excel file $destFile committed
</commit_message>
<xml_diff>
--- a/src/test/resources/NewExcel.xlsx
+++ b/src/test/resources/NewExcel.xlsx
@@ -8,12 +8,13 @@
   <sheets>
     <sheet name="Sheet1" r:id="rId3" sheetId="1"/>
     <sheet name="TestSheet" r:id="rId4" sheetId="2"/>
+    <sheet name="csvtest" r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="31">
   <si>
     <t>element_type</t>
   </si>
@@ -103,6 +104,9 @@
   </si>
   <si>
     <t>row1</t>
+  </si>
+  <si>
+    <t>csv</t>
   </si>
 </sst>
 </file>
@@ -332,4 +336,33 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>